<commit_message>
shiftDate gets assigned to corresponding day in excel file
</commit_message>
<xml_diff>
--- a/Server/assets/empty_report.xlsx
+++ b/Server/assets/empty_report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\OneDrive\Desktop\Schule\4. Klasse\PRE\_project\PRE2024-25\Server\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B01799-901B-43D2-B67F-3B4F8ECD85E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0351AE5-E862-4770-86F2-3B1F52903C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -774,11 +774,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1003,6 +1027,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1350,10 +1383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U39"/>
+  <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2197,7 +2230,7 @@
       <c r="G31" s="73"/>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
-      <c r="J31" s="74">
+      <c r="J31" s="76">
         <v>0</v>
       </c>
       <c r="K31" s="34"/>
@@ -2216,15 +2249,6 @@
     </row>
     <row r="32" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E32" s="47"/>
-      <c r="F32" s="46"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="J32" s="75">
-        <f>SUM(J4:J31)</f>
-        <v>0</v>
-      </c>
       <c r="Q32" s="59">
         <f>SUM(Q4:Q31)</f>
         <v>0</v>
@@ -2236,11 +2260,7 @@
     </row>
     <row r="33" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E33" s="47"/>
-      <c r="F33" s="48"/>
-      <c r="I33" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="J33" s="5"/>
+      <c r="G33" s="78"/>
       <c r="Q33" s="44"/>
       <c r="R33" s="61">
         <f>SUM(Q32:R32)</f>
@@ -2249,68 +2269,104 @@
     </row>
     <row r="34" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E34" s="47"/>
-      <c r="F34" s="48"/>
-      <c r="I34" s="54" t="s">
+      <c r="I34" s="78"/>
+    </row>
+    <row r="35" spans="1:18" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="47"/>
+    </row>
+    <row r="36" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="47"/>
+    </row>
+    <row r="37" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E37" s="47"/>
+    </row>
+    <row r="38" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F40" s="46"/>
+      <c r="G40" s="77"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="J40" s="75">
+        <f>SUM(J4:J31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F41" s="48"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="36"/>
+      <c r="C42" s="38">
+        <v>30</v>
+      </c>
+      <c r="F42" s="48"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="1:18" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="36"/>
-      <c r="C35" s="38">
-        <v>30</v>
-      </c>
-      <c r="E35" s="47"/>
-      <c r="F35" s="49"/>
-      <c r="I35" s="55" t="s">
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="22"/>
+      <c r="C43" s="32"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="22"/>
-      <c r="C36" s="32"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="50"/>
-      <c r="I36" s="56" t="s">
+      <c r="J43" s="5"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="42"/>
+      <c r="C44" s="32"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="J36" s="5"/>
-    </row>
-    <row r="37" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="42"/>
-      <c r="C37" s="32"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="57" t="s">
+      <c r="J44" s="5"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="43"/>
+      <c r="C45" s="32"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="J37" s="6"/>
-    </row>
-    <row r="38" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" s="43"/>
-      <c r="C38" s="32"/>
-    </row>
-    <row r="39" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="41" t="s">
+      <c r="J45" s="6"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="6"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>